<commit_message>
add code in contact
</commit_message>
<xml_diff>
--- a/assets/format.xlsx
+++ b/assets/format.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS VivoBook\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F0540A62-7026-4B59-810C-963C47F05D7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A91DDC5C-2F8D-4847-9517-EB7766408576}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{A03CBE7E-084A-440F-AC9B-3E8EA4CFE469}"/>
+    <workbookView xWindow="3780" yWindow="3555" windowWidth="21600" windowHeight="11295" xr2:uid="{A03CBE7E-084A-440F-AC9B-3E8EA4CFE469}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>No</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>No. WA</t>
+  </si>
+  <si>
+    <t>Kode</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37AA750-63FE-4A0A-9F46-6740EA87D607}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,7 +407,7 @@
     <col min="3" max="3" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,6 +417,9 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>